<commit_message>
Removed Trailing Zeroes, added LaTeX parsing
NumberCard class now contains methods to generate LaTeX code,  AskAnswer
during practice mode now generates LaTeX images with jlatex library.

Trailing zeroes in cards during decimal mode and the score display are
now removed with the new truncZeros method
</commit_message>
<xml_diff>
--- a/src/spreadsheets/Decimals.xlsx
+++ b/src/spreadsheets/Decimals.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Google Drive\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="7200"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,6 +38,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.###"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -71,8 +70,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -355,32 +355,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="M67" sqref="M67"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E28" activeCellId="2" sqref="B1:B1048576 D1:D1048576 E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
-      <c r="B1">
+      <c r="B1" s="1">
         <v>9.4</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1">
+      <c r="D1" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>14.5</v>
       </c>
     </row>
@@ -388,16 +388,16 @@
       <c r="A2">
         <v>2</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>8.8000000000000007</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>8.6999999999999993</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>17.5</v>
       </c>
     </row>
@@ -405,16 +405,16 @@
       <c r="A3">
         <v>3</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>9.8000000000000007</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="1">
         <v>5.0999999999999996</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="1">
         <v>14.9</v>
       </c>
     </row>
@@ -422,16 +422,16 @@
       <c r="A4">
         <v>4</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>8</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="1">
         <v>8.6</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="1">
         <v>16.600000000000001</v>
       </c>
     </row>
@@ -439,16 +439,16 @@
       <c r="A5">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>1.8</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>1.4</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="1">
         <v>3.2</v>
       </c>
     </row>
@@ -456,16 +456,16 @@
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>3.7</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="1">
         <v>3.8</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="1">
         <v>7.5</v>
       </c>
     </row>
@@ -473,16 +473,16 @@
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>6.9</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="1">
         <v>5.2</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="1">
         <v>12.1</v>
       </c>
     </row>
@@ -490,16 +490,16 @@
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>3.8</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="1">
         <v>6.1</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="1">
         <v>9.9</v>
       </c>
     </row>
@@ -507,16 +507,16 @@
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>7.8</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="1">
         <v>8.1</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="1">
         <v>15.9</v>
       </c>
     </row>
@@ -524,16 +524,16 @@
       <c r="A10">
         <v>10</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>1.7</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="1">
         <v>10.5</v>
       </c>
     </row>
@@ -541,16 +541,16 @@
       <c r="A11">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>5.6</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="1">
         <v>1.3</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="1">
         <v>6.9</v>
       </c>
     </row>
@@ -558,16 +558,16 @@
       <c r="A12">
         <v>12</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>0.6</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="1">
         <v>4.7</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="1">
         <v>5.3</v>
       </c>
     </row>
@@ -575,16 +575,16 @@
       <c r="A13">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>3.39</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="1">
         <v>3.37</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="1">
         <v>6.76</v>
       </c>
     </row>
@@ -592,16 +592,16 @@
       <c r="A14">
         <v>14</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>7.31</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="1">
         <v>2.69</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="1">
         <v>10</v>
       </c>
     </row>
@@ -609,16 +609,16 @@
       <c r="A15">
         <v>15</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>6.14</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>2.06</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>8.1999999999999993</v>
       </c>
     </row>
@@ -626,16 +626,16 @@
       <c r="A16">
         <v>16</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>4.84</v>
       </c>
       <c r="C16" t="s">
         <v>0</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="1">
         <v>4.05</v>
       </c>
-      <c r="E16">
+      <c r="E16" s="1">
         <v>8.89</v>
       </c>
     </row>
@@ -643,16 +643,16 @@
       <c r="A17">
         <v>17</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>6.47</v>
       </c>
       <c r="C17" t="s">
         <v>0</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="1">
         <v>7.98</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="1">
         <v>14.45</v>
       </c>
     </row>
@@ -660,16 +660,16 @@
       <c r="A18">
         <v>18</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>2.08</v>
       </c>
       <c r="C18" t="s">
         <v>0</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="1">
         <v>8.19</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="1">
         <v>10.27</v>
       </c>
     </row>
@@ -677,16 +677,16 @@
       <c r="A19">
         <v>19</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>0.98</v>
       </c>
       <c r="C19" t="s">
         <v>0</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="1">
         <v>6.29</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="1">
         <v>7.27</v>
       </c>
     </row>
@@ -694,16 +694,16 @@
       <c r="A20">
         <v>20</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>6.17</v>
       </c>
       <c r="C20" t="s">
         <v>0</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="1">
         <v>4.4400000000000004</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="1">
         <v>10.61</v>
       </c>
     </row>
@@ -711,16 +711,16 @@
       <c r="A21">
         <v>21</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>1.38</v>
       </c>
       <c r="C21" t="s">
         <v>0</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="1">
         <v>9.1300000000000008</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="1">
         <v>10.51</v>
       </c>
     </row>
@@ -728,16 +728,16 @@
       <c r="A22">
         <v>22</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="1">
         <v>4.6399999999999997</v>
       </c>
       <c r="C22" t="s">
         <v>0</v>
       </c>
-      <c r="D22">
+      <c r="D22" s="1">
         <v>3.89</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="1">
         <v>8.5299999999999994</v>
       </c>
     </row>
@@ -745,16 +745,16 @@
       <c r="A23">
         <v>23</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="1">
         <v>5.93</v>
       </c>
       <c r="C23" t="s">
         <v>0</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>5.0599999999999996</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>10.99</v>
       </c>
     </row>
@@ -762,16 +762,16 @@
       <c r="A24">
         <v>24</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="1">
         <v>0.91</v>
       </c>
       <c r="C24" t="s">
         <v>0</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="1">
         <v>0.34</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="1">
         <v>1.25</v>
       </c>
     </row>
@@ -779,16 +779,16 @@
       <c r="A25">
         <v>25</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="1">
         <v>4.3899999999999997</v>
       </c>
       <c r="C25" t="s">
         <v>0</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="1">
         <v>0.86</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="1">
         <v>5.25</v>
       </c>
     </row>
@@ -796,16 +796,16 @@
       <c r="A26">
         <v>26</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <v>6.15</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="1">
         <v>0.98</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="1">
         <v>5.17</v>
       </c>
     </row>
@@ -813,16 +813,16 @@
       <c r="A27">
         <v>27</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <v>7.36</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="1">
         <v>7.28</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="1">
         <v>0.08</v>
       </c>
     </row>
@@ -830,16 +830,16 @@
       <c r="A28">
         <v>28</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <v>0.32</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="1">
         <v>0.25</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -847,16 +847,16 @@
       <c r="A29">
         <v>29</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <v>7.89</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="1">
         <v>3.26</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="1">
         <v>4.63</v>
       </c>
     </row>
@@ -864,16 +864,16 @@
       <c r="A30">
         <v>30</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <v>0.82</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="1">
         <v>0.25</v>
       </c>
     </row>
@@ -881,16 +881,16 @@
       <c r="A31">
         <v>31</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <v>4.3099999999999996</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="1">
         <v>2.4300000000000002</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="1">
         <v>1.88</v>
       </c>
     </row>
@@ -898,16 +898,16 @@
       <c r="A32">
         <v>32</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="1">
         <v>3.55</v>
       </c>
       <c r="C32" t="s">
         <v>1</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="1">
         <v>0.79</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="1">
         <v>2.76</v>
       </c>
     </row>
@@ -915,16 +915,16 @@
       <c r="A33">
         <v>33</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="1">
         <v>2.46</v>
       </c>
       <c r="C33" t="s">
         <v>1</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="1">
         <v>0.32</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="1">
         <v>2.14</v>
       </c>
     </row>
@@ -932,16 +932,16 @@
       <c r="A34">
         <v>34</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="1">
         <v>5.2</v>
       </c>
       <c r="C34" t="s">
         <v>1</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="1">
         <v>1.26</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="1">
         <v>3.94</v>
       </c>
     </row>
@@ -949,16 +949,16 @@
       <c r="A35">
         <v>35</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="1">
         <v>3.41</v>
       </c>
       <c r="C35" t="s">
         <v>1</v>
       </c>
-      <c r="D35">
+      <c r="D35" s="1">
         <v>0.27</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="1">
         <v>3.14</v>
       </c>
     </row>
@@ -966,16 +966,16 @@
       <c r="A36">
         <v>36</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="1">
         <v>2.35</v>
       </c>
       <c r="C36" t="s">
         <v>1</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="1">
         <v>0.24</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="1">
         <v>2.11</v>
       </c>
     </row>
@@ -983,16 +983,16 @@
       <c r="A37">
         <v>37</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="1">
         <v>2.25</v>
       </c>
       <c r="C37" t="s">
         <v>1</v>
       </c>
-      <c r="D37">
+      <c r="D37" s="1">
         <v>0.82</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="1">
         <v>1.43</v>
       </c>
     </row>
@@ -1000,16 +1000,16 @@
       <c r="A38">
         <v>38</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="1">
         <v>1.76</v>
       </c>
       <c r="C38" t="s">
         <v>1</v>
       </c>
-      <c r="D38">
+      <c r="D38" s="1">
         <v>1.34</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="1">
         <v>0.42</v>
       </c>
     </row>
@@ -1017,16 +1017,16 @@
       <c r="A39">
         <v>39</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="1">
         <v>7.9</v>
       </c>
       <c r="C39" t="s">
         <v>1</v>
       </c>
-      <c r="D39">
+      <c r="D39" s="1">
         <v>2.5499999999999998</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="1">
         <v>5.35</v>
       </c>
     </row>
@@ -1034,16 +1034,16 @@
       <c r="A40">
         <v>40</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="1">
         <v>3.06</v>
       </c>
       <c r="C40" t="s">
         <v>1</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="1">
         <v>0.11</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="1">
         <v>2.95</v>
       </c>
     </row>
@@ -1051,16 +1051,16 @@
       <c r="A41">
         <v>41</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="1">
         <v>1.94</v>
       </c>
       <c r="C41" t="s">
         <v>1</v>
       </c>
-      <c r="D41">
+      <c r="D41" s="1">
         <v>0.4</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="1">
         <v>1.54</v>
       </c>
     </row>
@@ -1068,16 +1068,16 @@
       <c r="A42">
         <v>42</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="1">
         <v>6.15</v>
       </c>
       <c r="C42" t="s">
         <v>1</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="1">
         <v>0.98</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="1">
         <v>5.17</v>
       </c>
     </row>
@@ -1085,16 +1085,16 @@
       <c r="A43">
         <v>43</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="1">
         <v>7.36</v>
       </c>
       <c r="C43" t="s">
         <v>1</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="1">
         <v>7.28</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="1">
         <v>0.08</v>
       </c>
     </row>
@@ -1102,16 +1102,16 @@
       <c r="A44">
         <v>44</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="1">
         <v>0.32</v>
       </c>
       <c r="C44" t="s">
         <v>1</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="1">
         <v>0.25</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="1">
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
@@ -1119,16 +1119,16 @@
       <c r="A45">
         <v>45</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="1">
         <v>7.89</v>
       </c>
       <c r="C45" t="s">
         <v>1</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="1">
         <v>3.26</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="1">
         <v>4.63</v>
       </c>
     </row>
@@ -1136,16 +1136,16 @@
       <c r="A46">
         <v>46</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="1">
         <v>0.82</v>
       </c>
       <c r="C46" t="s">
         <v>1</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="1">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="1">
         <v>0.25</v>
       </c>
     </row>
@@ -1153,16 +1153,16 @@
       <c r="A47">
         <v>47</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="1">
         <v>4.3099999999999996</v>
       </c>
       <c r="C47" t="s">
         <v>1</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="1">
         <v>2.4300000000000002</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="1">
         <v>1.88</v>
       </c>
     </row>
@@ -1170,16 +1170,16 @@
       <c r="A48">
         <v>48</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="1">
         <v>5.2</v>
       </c>
       <c r="C48" t="s">
         <v>1</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="1">
         <v>1.26</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="1">
         <v>3.94</v>
       </c>
     </row>
@@ -1187,16 +1187,16 @@
       <c r="A49">
         <v>49</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="1">
         <v>3.41</v>
       </c>
       <c r="C49" t="s">
         <v>1</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="1">
         <v>0.27</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="1">
         <v>3.14</v>
       </c>
     </row>
@@ -1204,16 +1204,16 @@
       <c r="A50">
         <v>50</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="1">
         <v>2.35</v>
       </c>
       <c r="C50" t="s">
         <v>1</v>
       </c>
-      <c r="D50">
+      <c r="D50" s="1">
         <v>0.24</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="1">
         <v>2.11</v>
       </c>
     </row>
@@ -1221,16 +1221,16 @@
       <c r="A51">
         <v>51</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="1">
         <v>1.81</v>
       </c>
       <c r="C51" t="s">
         <v>2</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="1">
         <v>7.94</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="1">
         <f>B51*D51</f>
         <v>14.371400000000001</v>
       </c>
@@ -1239,16 +1239,16 @@
       <c r="A52">
         <v>52</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="1">
         <v>8.7200000000000006</v>
       </c>
       <c r="C52" t="s">
         <v>2</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="1">
         <v>0.15</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="1">
         <f t="shared" ref="E52:E74" si="0">B52*D52</f>
         <v>1.3080000000000001</v>
       </c>
@@ -1257,16 +1257,16 @@
       <c r="A53">
         <v>53</v>
       </c>
-      <c r="B53">
+      <c r="B53" s="1">
         <v>2.2400000000000002</v>
       </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
-      <c r="D53">
+      <c r="D53" s="1">
         <v>8.8000000000000007</v>
       </c>
-      <c r="E53">
+      <c r="E53" s="1">
         <f t="shared" si="0"/>
         <v>19.712000000000003</v>
       </c>
@@ -1275,16 +1275,16 @@
       <c r="A54">
         <v>54</v>
       </c>
-      <c r="B54">
+      <c r="B54" s="1">
         <v>1.39</v>
       </c>
       <c r="C54" t="s">
         <v>2</v>
       </c>
-      <c r="D54">
+      <c r="D54" s="1">
         <v>0.09</v>
       </c>
-      <c r="E54">
+      <c r="E54" s="1">
         <f t="shared" si="0"/>
         <v>0.12509999999999999</v>
       </c>
@@ -1293,16 +1293,16 @@
       <c r="A55">
         <v>55</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="1">
         <v>5.87</v>
       </c>
       <c r="C55" t="s">
         <v>2</v>
       </c>
-      <c r="D55">
+      <c r="D55" s="1">
         <v>3.54</v>
       </c>
-      <c r="E55">
+      <c r="E55" s="1">
         <f t="shared" si="0"/>
         <v>20.779800000000002</v>
       </c>
@@ -1311,16 +1311,16 @@
       <c r="A56">
         <v>56</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="1">
         <v>9.02</v>
       </c>
       <c r="C56" t="s">
         <v>2</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="1">
         <v>4.2</v>
       </c>
-      <c r="E56">
+      <c r="E56" s="1">
         <f t="shared" si="0"/>
         <v>37.884</v>
       </c>
@@ -1329,16 +1329,16 @@
       <c r="A57">
         <v>57</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="1">
         <v>4.4000000000000004</v>
       </c>
       <c r="C57" t="s">
         <v>2</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="1">
         <v>6.38</v>
       </c>
-      <c r="E57">
+      <c r="E57" s="1">
         <f t="shared" si="0"/>
         <v>28.072000000000003</v>
       </c>
@@ -1347,16 +1347,16 @@
       <c r="A58">
         <v>58</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="1">
         <v>7.18</v>
       </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
-      <c r="D58">
+      <c r="D58" s="1">
         <v>3.44</v>
       </c>
-      <c r="E58">
+      <c r="E58" s="1">
         <f t="shared" si="0"/>
         <v>24.699199999999998</v>
       </c>
@@ -1365,16 +1365,16 @@
       <c r="A59">
         <v>59</v>
       </c>
-      <c r="B59">
+      <c r="B59" s="1">
         <v>5.74</v>
       </c>
       <c r="C59" t="s">
         <v>2</v>
       </c>
-      <c r="D59">
+      <c r="D59" s="1">
         <v>4.37</v>
       </c>
-      <c r="E59">
+      <c r="E59" s="1">
         <f t="shared" si="0"/>
         <v>25.0838</v>
       </c>
@@ -1383,16 +1383,16 @@
       <c r="A60">
         <v>60</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="1">
         <v>0.56000000000000005</v>
       </c>
       <c r="C60" t="s">
         <v>2</v>
       </c>
-      <c r="D60">
+      <c r="D60" s="1">
         <v>9.23</v>
       </c>
-      <c r="E60">
+      <c r="E60" s="1">
         <f t="shared" si="0"/>
         <v>5.1688000000000009</v>
       </c>
@@ -1401,16 +1401,16 @@
       <c r="A61">
         <v>61</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="1">
         <v>6.19</v>
       </c>
       <c r="C61" t="s">
         <v>2</v>
       </c>
-      <c r="D61">
+      <c r="D61" s="1">
         <v>6.59</v>
       </c>
-      <c r="E61">
+      <c r="E61" s="1">
         <f t="shared" si="0"/>
         <v>40.792100000000005</v>
       </c>
@@ -1419,16 +1419,16 @@
       <c r="A62">
         <v>62</v>
       </c>
-      <c r="B62">
+      <c r="B62" s="1">
         <v>1.28</v>
       </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
-      <c r="D62">
+      <c r="D62" s="1">
         <v>6.65</v>
       </c>
-      <c r="E62">
+      <c r="E62" s="1">
         <f t="shared" si="0"/>
         <v>8.5120000000000005</v>
       </c>
@@ -1437,16 +1437,16 @@
       <c r="A63">
         <v>63</v>
       </c>
-      <c r="B63">
+      <c r="B63" s="1">
         <v>1.39</v>
       </c>
       <c r="C63" t="s">
         <v>2</v>
       </c>
-      <c r="D63">
+      <c r="D63" s="1">
         <v>0.34</v>
       </c>
-      <c r="E63">
+      <c r="E63" s="1">
         <f t="shared" si="0"/>
         <v>0.47260000000000002</v>
       </c>
@@ -1455,16 +1455,16 @@
       <c r="A64">
         <v>64</v>
       </c>
-      <c r="B64">
+      <c r="B64" s="1">
         <v>1.58</v>
       </c>
       <c r="C64" t="s">
         <v>2</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="1">
         <v>0.53</v>
       </c>
-      <c r="E64">
+      <c r="E64" s="1">
         <f t="shared" si="0"/>
         <v>0.83740000000000003</v>
       </c>
@@ -1473,16 +1473,16 @@
       <c r="A65">
         <v>65</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="1">
         <v>1.58</v>
       </c>
       <c r="C65" t="s">
         <v>2</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="1">
         <v>2.75</v>
       </c>
-      <c r="E65">
+      <c r="E65" s="1">
         <f t="shared" si="0"/>
         <v>4.3450000000000006</v>
       </c>
@@ -1491,16 +1491,16 @@
       <c r="A66">
         <v>66</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="1">
         <v>2.73</v>
       </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="1">
         <v>2.94</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="1">
         <f t="shared" si="0"/>
         <v>8.0261999999999993</v>
       </c>
@@ -1509,16 +1509,16 @@
       <c r="A67">
         <v>67</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="1">
         <v>0.35</v>
       </c>
       <c r="C67" t="s">
         <v>2</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="1">
         <v>1.02</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="1">
         <f t="shared" si="0"/>
         <v>0.35699999999999998</v>
       </c>
@@ -1527,16 +1527,16 @@
       <c r="A68">
         <v>68</v>
       </c>
-      <c r="B68">
+      <c r="B68" s="1">
         <v>0.64</v>
       </c>
       <c r="C68" t="s">
         <v>2</v>
       </c>
-      <c r="D68">
+      <c r="D68" s="1">
         <v>1.51</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="1">
         <f t="shared" si="0"/>
         <v>0.96640000000000004</v>
       </c>
@@ -1545,16 +1545,16 @@
       <c r="A69">
         <v>69</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="1">
         <v>2.67</v>
       </c>
       <c r="C69" t="s">
         <v>2</v>
       </c>
-      <c r="D69">
+      <c r="D69" s="1">
         <v>0.5</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="1">
         <f t="shared" si="0"/>
         <v>1.335</v>
       </c>
@@ -1563,16 +1563,16 @@
       <c r="A70">
         <v>70</v>
       </c>
-      <c r="B70">
+      <c r="B70" s="1">
         <v>0.79</v>
       </c>
       <c r="C70" t="s">
         <v>2</v>
       </c>
-      <c r="D70">
+      <c r="D70" s="1">
         <v>0.94</v>
       </c>
-      <c r="E70">
+      <c r="E70" s="1">
         <f t="shared" si="0"/>
         <v>0.74260000000000004</v>
       </c>
@@ -1581,16 +1581,16 @@
       <c r="A71">
         <v>71</v>
       </c>
-      <c r="B71">
+      <c r="B71" s="1">
         <v>0.51</v>
       </c>
       <c r="C71" t="s">
         <v>2</v>
       </c>
-      <c r="D71">
+      <c r="D71" s="1">
         <v>2.58</v>
       </c>
-      <c r="E71">
+      <c r="E71" s="1">
         <f t="shared" si="0"/>
         <v>1.3158000000000001</v>
       </c>
@@ -1599,16 +1599,16 @@
       <c r="A72">
         <v>72</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="1">
         <v>0.28000000000000003</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>
-      <c r="D72">
+      <c r="D72" s="1">
         <v>0.22</v>
       </c>
-      <c r="E72">
+      <c r="E72" s="1">
         <f t="shared" si="0"/>
         <v>6.1600000000000009E-2</v>
       </c>
@@ -1617,16 +1617,16 @@
       <c r="A73">
         <v>73</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="1">
         <v>0.67</v>
       </c>
       <c r="C73" t="s">
         <v>2</v>
       </c>
-      <c r="D73">
+      <c r="D73" s="1">
         <v>1.57</v>
       </c>
-      <c r="E73">
+      <c r="E73" s="1">
         <f t="shared" si="0"/>
         <v>1.0519000000000001</v>
       </c>
@@ -1635,16 +1635,16 @@
       <c r="A74">
         <v>74</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="1">
         <v>1.2</v>
       </c>
       <c r="C74" t="s">
         <v>2</v>
       </c>
-      <c r="D74">
+      <c r="D74" s="1">
         <v>2.92</v>
       </c>
-      <c r="E74">
+      <c r="E74" s="1">
         <f t="shared" si="0"/>
         <v>3.504</v>
       </c>
@@ -1653,16 +1653,16 @@
       <c r="A75">
         <v>75</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="1">
         <v>1.05</v>
       </c>
       <c r="C75" t="s">
         <v>2</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="1">
         <v>1.76</v>
       </c>
-      <c r="E75">
+      <c r="E75" s="1">
         <f>B75*D75</f>
         <v>1.8480000000000001</v>
       </c>
@@ -1671,16 +1671,16 @@
       <c r="A76">
         <v>76</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="1">
         <v>8.8000000000000007</v>
       </c>
       <c r="C76" t="s">
         <v>3</v>
       </c>
-      <c r="D76">
-        <v>2</v>
-      </c>
-      <c r="E76">
+      <c r="D76" s="1">
+        <v>2</v>
+      </c>
+      <c r="E76" s="1">
         <f>B76/D76</f>
         <v>4.4000000000000004</v>
       </c>
@@ -1689,16 +1689,16 @@
       <c r="A77">
         <v>77</v>
       </c>
-      <c r="B77">
+      <c r="B77" s="1">
         <v>40.5</v>
       </c>
       <c r="C77" t="s">
         <v>3</v>
       </c>
-      <c r="D77">
+      <c r="D77" s="1">
         <v>5</v>
       </c>
-      <c r="E77">
+      <c r="E77" s="1">
         <f t="shared" ref="E77:E100" si="1">B77/D77</f>
         <v>8.1</v>
       </c>
@@ -1707,16 +1707,16 @@
       <c r="A78">
         <v>78</v>
       </c>
-      <c r="B78">
+      <c r="B78" s="1">
         <v>64.8</v>
       </c>
       <c r="C78" t="s">
         <v>3</v>
       </c>
-      <c r="D78">
+      <c r="D78" s="1">
         <v>64.8</v>
       </c>
-      <c r="E78">
+      <c r="E78" s="1">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
@@ -1725,16 +1725,16 @@
       <c r="A79">
         <v>79</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="1">
         <v>81.3</v>
       </c>
       <c r="C79" t="s">
         <v>3</v>
       </c>
-      <c r="D79">
-        <v>3</v>
-      </c>
-      <c r="E79">
+      <c r="D79" s="1">
+        <v>3</v>
+      </c>
+      <c r="E79" s="1">
         <f t="shared" si="1"/>
         <v>27.099999999999998</v>
       </c>
@@ -1743,16 +1743,16 @@
       <c r="A80">
         <v>80</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="1">
         <v>24.8</v>
       </c>
       <c r="C80" t="s">
         <v>3</v>
       </c>
-      <c r="D80">
+      <c r="D80" s="1">
         <v>4</v>
       </c>
-      <c r="E80">
+      <c r="E80" s="1">
         <f t="shared" si="1"/>
         <v>6.2</v>
       </c>
@@ -1761,16 +1761,16 @@
       <c r="A81">
         <v>81</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="1">
         <v>48.8</v>
       </c>
       <c r="C81" t="s">
         <v>3</v>
       </c>
-      <c r="D81">
-        <v>2</v>
-      </c>
-      <c r="E81">
+      <c r="D81" s="1">
+        <v>2</v>
+      </c>
+      <c r="E81" s="1">
         <f t="shared" si="1"/>
         <v>24.4</v>
       </c>
@@ -1779,16 +1779,16 @@
       <c r="A82">
         <v>82</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="1">
         <v>12.6</v>
       </c>
       <c r="C82" t="s">
         <v>3</v>
       </c>
-      <c r="D82">
-        <v>3</v>
-      </c>
-      <c r="E82">
+      <c r="D82" s="1">
+        <v>3</v>
+      </c>
+      <c r="E82" s="1">
         <f t="shared" si="1"/>
         <v>4.2</v>
       </c>
@@ -1797,16 +1797,16 @@
       <c r="A83">
         <v>83</v>
       </c>
-      <c r="B83">
+      <c r="B83" s="1">
         <v>44.6</v>
       </c>
       <c r="C83" t="s">
         <v>3</v>
       </c>
-      <c r="D83">
-        <v>2</v>
-      </c>
-      <c r="E83">
+      <c r="D83" s="1">
+        <v>2</v>
+      </c>
+      <c r="E83" s="1">
         <f t="shared" si="1"/>
         <v>22.3</v>
       </c>
@@ -1815,16 +1815,16 @@
       <c r="A84">
         <v>84</v>
       </c>
-      <c r="B84">
+      <c r="B84" s="1">
         <v>48.8</v>
       </c>
       <c r="C84" t="s">
         <v>3</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="1">
         <v>8</v>
       </c>
-      <c r="E84">
+      <c r="E84" s="1">
         <f t="shared" si="1"/>
         <v>6.1</v>
       </c>
@@ -1833,16 +1833,16 @@
       <c r="A85">
         <v>85</v>
       </c>
-      <c r="B85">
+      <c r="B85" s="1">
         <v>6.6</v>
       </c>
       <c r="C85" t="s">
         <v>3</v>
       </c>
-      <c r="D85">
-        <v>2</v>
-      </c>
-      <c r="E85">
+      <c r="D85" s="1">
+        <v>2</v>
+      </c>
+      <c r="E85" s="1">
         <f t="shared" si="1"/>
         <v>3.3</v>
       </c>
@@ -1851,16 +1851,16 @@
       <c r="A86">
         <v>86</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="1">
         <v>36.799999999999997</v>
       </c>
       <c r="C86" t="s">
         <v>3</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="1">
         <v>4</v>
       </c>
-      <c r="E86">
+      <c r="E86" s="1">
         <f t="shared" si="1"/>
         <v>9.1999999999999993</v>
       </c>
@@ -1869,16 +1869,16 @@
       <c r="A87">
         <v>87</v>
       </c>
-      <c r="B87">
+      <c r="B87" s="1">
         <v>9.6</v>
       </c>
       <c r="C87" t="s">
         <v>3</v>
       </c>
-      <c r="D87">
-        <v>3</v>
-      </c>
-      <c r="E87">
+      <c r="D87" s="1">
+        <v>3</v>
+      </c>
+      <c r="E87" s="1">
         <f t="shared" si="1"/>
         <v>3.1999999999999997</v>
       </c>
@@ -1887,16 +1887,16 @@
       <c r="A88">
         <v>88</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="1">
         <v>14.6</v>
       </c>
       <c r="C88" t="s">
         <v>3</v>
       </c>
-      <c r="D88">
-        <v>2</v>
-      </c>
-      <c r="E88">
+      <c r="D88" s="1">
+        <v>2</v>
+      </c>
+      <c r="E88" s="1">
         <f t="shared" si="1"/>
         <v>7.3</v>
       </c>
@@ -1905,16 +1905,16 @@
       <c r="A89">
         <v>89</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="1">
         <v>48.6</v>
       </c>
       <c r="C89" t="s">
         <v>3</v>
       </c>
-      <c r="D89">
+      <c r="D89" s="1">
         <v>6</v>
       </c>
-      <c r="E89">
+      <c r="E89" s="1">
         <f t="shared" si="1"/>
         <v>8.1</v>
       </c>
@@ -1923,16 +1923,16 @@
       <c r="A90">
         <v>90</v>
       </c>
-      <c r="B90">
+      <c r="B90" s="1">
         <v>18.8</v>
       </c>
       <c r="C90" t="s">
         <v>3</v>
       </c>
-      <c r="D90">
-        <v>2</v>
-      </c>
-      <c r="E90">
+      <c r="D90" s="1">
+        <v>2</v>
+      </c>
+      <c r="E90" s="1">
         <f t="shared" si="1"/>
         <v>9.4</v>
       </c>
@@ -1941,16 +1941,16 @@
       <c r="A91">
         <v>91</v>
       </c>
-      <c r="B91">
+      <c r="B91" s="1">
         <v>32.799999999999997</v>
       </c>
       <c r="C91" t="s">
         <v>3</v>
       </c>
-      <c r="D91">
+      <c r="D91" s="1">
         <v>8</v>
       </c>
-      <c r="E91">
+      <c r="E91" s="1">
         <f t="shared" si="1"/>
         <v>4.0999999999999996</v>
       </c>
@@ -1959,16 +1959,16 @@
       <c r="A92">
         <v>92</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="1">
         <v>96.42</v>
       </c>
       <c r="C92" t="s">
         <v>3</v>
       </c>
-      <c r="D92">
+      <c r="D92" s="1">
         <v>10</v>
       </c>
-      <c r="E92">
+      <c r="E92" s="1">
         <f t="shared" si="1"/>
         <v>9.6419999999999995</v>
       </c>
@@ -1977,16 +1977,16 @@
       <c r="A93">
         <v>93</v>
       </c>
-      <c r="B93">
+      <c r="B93" s="1">
         <v>0.3</v>
       </c>
       <c r="C93" t="s">
         <v>3</v>
       </c>
-      <c r="D93">
+      <c r="D93" s="1">
         <v>10</v>
       </c>
-      <c r="E93">
+      <c r="E93" s="1">
         <f t="shared" si="1"/>
         <v>0.03</v>
       </c>
@@ -1995,16 +1995,16 @@
       <c r="A94">
         <v>94</v>
       </c>
-      <c r="B94">
+      <c r="B94" s="1">
         <v>15.12</v>
       </c>
       <c r="C94" t="s">
         <v>3</v>
       </c>
-      <c r="D94">
+      <c r="D94" s="1">
         <v>2.4</v>
       </c>
-      <c r="E94">
+      <c r="E94" s="1">
         <f t="shared" si="1"/>
         <v>6.3</v>
       </c>
@@ -2013,16 +2013,16 @@
       <c r="A95">
         <v>95</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="1">
         <v>18.149999999999999</v>
       </c>
       <c r="C95" t="s">
         <v>3</v>
       </c>
-      <c r="D95">
+      <c r="D95" s="1">
         <v>1.5</v>
       </c>
-      <c r="E95">
+      <c r="E95" s="1">
         <f t="shared" si="1"/>
         <v>12.1</v>
       </c>
@@ -2031,16 +2031,16 @@
       <c r="A96">
         <v>96</v>
       </c>
-      <c r="B96">
+      <c r="B96" s="1">
         <v>8.82</v>
       </c>
       <c r="C96" t="s">
         <v>3</v>
       </c>
-      <c r="D96">
+      <c r="D96" s="1">
         <v>1.8</v>
       </c>
-      <c r="E96">
+      <c r="E96" s="1">
         <f t="shared" si="1"/>
         <v>4.9000000000000004</v>
       </c>
@@ -2049,16 +2049,16 @@
       <c r="A97">
         <v>97</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="1">
         <v>283.5</v>
       </c>
       <c r="C97" t="s">
         <v>3</v>
       </c>
-      <c r="D97">
+      <c r="D97" s="1">
         <v>8.1</v>
       </c>
-      <c r="E97">
+      <c r="E97" s="1">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
@@ -2067,16 +2067,16 @@
       <c r="A98">
         <v>98</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="1">
         <v>75.959999999999994</v>
       </c>
       <c r="C98" t="s">
         <v>3</v>
       </c>
-      <c r="D98">
+      <c r="D98" s="1">
         <v>3.6</v>
       </c>
-      <c r="E98">
+      <c r="E98" s="1">
         <f t="shared" si="1"/>
         <v>21.099999999999998</v>
       </c>
@@ -2085,16 +2085,16 @@
       <c r="A99">
         <v>99</v>
       </c>
-      <c r="B99">
+      <c r="B99" s="1">
         <v>25</v>
       </c>
       <c r="C99" t="s">
         <v>3</v>
       </c>
-      <c r="D99">
+      <c r="D99" s="1">
         <v>2.5</v>
       </c>
-      <c r="E99">
+      <c r="E99" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -2103,16 +2103,16 @@
       <c r="A100">
         <v>100</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="1">
         <v>31.25</v>
       </c>
       <c r="C100" t="s">
         <v>3</v>
       </c>
-      <c r="D100">
+      <c r="D100" s="1">
         <v>2.5</v>
       </c>
-      <c r="E100">
+      <c r="E100" s="1">
         <f t="shared" si="1"/>
         <v>12.5</v>
       </c>

</xml_diff>